<commit_message>
Separated the code into file files and added mapping for the visual files
</commit_message>
<xml_diff>
--- a/Tools/Validation/reports.xlsx
+++ b/Tools/Validation/reports.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testmaq-my.sharepoint.com/personal/amany_maqsoftware_com/Documents/Desktop/Automation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testmaq-my.sharepoint.com/personal/amany_maqsoftware_com/Documents/Desktop/Automation-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="11_5E4D13B184AE82E30B8E4DA877D9216CB684C33E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09CD4910-8F16-4A1E-8AF6-6B7EEAD5522A}"/>
+  <xr:revisionPtr revIDLastSave="235" documentId="11_5E4D13B184AE82E30B8E4DA877D9216CB684C33E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FE0EF2A-5CFE-4D18-BA97-2754BFA960E8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,6 +183,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,7 +477,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>